<commit_message>
Hoàn thành tính năng nhâpj excel và xuất pdf
</commit_message>
<xml_diff>
--- a/history_output.xlsx
+++ b/history_output.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,116 +466,139 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>45791.57323114583</v>
+        <v>45805.47588245371</v>
       </c>
       <c r="B2" t="n">
-        <v>0.04394000046111814</v>
+        <v>0.03337472496505753</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Tăng trưởng dài hạn, Tính thanh khoản, Khả năng chống lạm phát, Rủi ro đầu tư</t>
+          <t>Ổn định giá, Tăng trưởng dài hạn, tieu chi khac</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Vàng, Ngoại tệ, Cổ phiếu, Trái phiếu</t>
+          <t>Vàng, Ngoại tệ, phuong an khac</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Vàng (0.2500), Cổ phiếu (0.2402), Ngoại tệ (0.2305), Trái phiếu (0.1339)</t>
+          <t>Vàng (0.3333), Ngoại tệ (0.3333), phuong an khac (0.3333)</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>45791.56929572917</v>
+        <v>45798.58740990741</v>
       </c>
       <c r="B3" t="n">
-        <v>0.03922752072654331</v>
+        <v>0.03337472496505753</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Ổn định giá, Tăng trưởng dài hạn, Tính thanh khoản, Khả năng chống lạm phát</t>
+          <t>Ổn định giá, Tính thanh khoản, Tăng trưởng dài hạn</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Ngoại tệ, Vàng, Cổ phiếu, Trái phiếu</t>
+          <t>Ngoại tệ, Cổ phiếu, Vàng</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Ngoại tệ (0.2500), Vàng (0.2262), Cổ phiếu (0.1872), Trái phiếu (0.1713)</t>
+          <t>Ngoại tệ (0.3333), Cổ phiếu (0.3333), Vàng (0.3333)</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>45791.56531056713</v>
+        <v>45798.58724861111</v>
       </c>
       <c r="B4" t="n">
-        <v>0.04690196759569773</v>
+        <v>0.03337472496505753</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Ổn định giá, Tăng trưởng dài hạn, Tính thanh khoản, Khả năng chống lạm phát</t>
+          <t>Ổn định giá, Tính thanh khoản, Tăng trưởng dài hạn</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Vàng, Ngoại tệ, Cổ phiếu, Trái phiếu</t>
+          <t>Ngoại tệ, Cổ phiếu, Vàng</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Vàng (0.2500), Ngoại tệ (0.2326), Cổ phiếu (0.1901), Trái phiếu (0.1778)</t>
+          <t>Ngoại tệ (0.3333), Cổ phiếu (0.3333), Vàng (0.3333)</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>45791.56321806713</v>
+        <v>45798.57278447917</v>
       </c>
       <c r="B5" t="n">
-        <v>0.0436947584033341</v>
+        <v>0.06390856373847034</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Tăng trưởng dài hạn, Ổn định giá, Khả năng chống lạm phát, Tính thanh khoản</t>
+          <t>Ổn định giá, Tăng trưởng dài hạn, Tính thanh khoản</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Ngoại tệ, Vàng, Trái phiếu, sdsd</t>
+          <t>Ngoại tệ, Vàng, Cổ phiếu</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Ngoại tệ (0.2500), Vàng (0.2349), Trái phiếu (0.2097), sdsd (0.1524)</t>
+          <t>Ngoại tệ (0.3333), Vàng (0.2884), Cổ phiếu (0.2196)</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>45791.55990496528</v>
+        <v>45798.56284561343</v>
       </c>
       <c r="B6" t="n">
-        <v>0.05066848902530368</v>
+        <v>0.03337472496505753</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Ổn định giá, Tăng trưởng dài hạn, Tính thanh khoản, Khả năng chống lạm phát</t>
+          <t>Ổn định giá, Tăng trưởng dài hạn, Tính thanh khoản</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Vàng, Ngoại tệ, Cổ phiếu, Trái phiếu</t>
+          <t>Ngoại tệ, Vàng, Cổ phiếu</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Vàng (0.2500), Ngoại tệ (0.2242), Cổ phiếu (0.1855), Trái phiếu (0.1565)</t>
+          <t>Cổ phiếu (0.3832), Ngoại tệ (0.3333), Vàng (0.2879)</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="n">
+        <v>45798.55942474537</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0.03337472496505753</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Ổn định giá, Tăng trưởng dài hạn, Khả năng chống lạm phát</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Vàng, Ngoại tệ, Cổ phiếu</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Vàng (0.3333), Ngoại tệ (0.2771), Cổ phiếu (0.2406)</t>
         </is>
       </c>
     </row>

</xml_diff>